<commit_message>
refactor: move algos to folders
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>Prime Image</t>
   </si>
@@ -196,6 +196,60 @@
   </si>
   <si>
     <t>iteration_9_arnold.jpg</t>
+  </si>
+  <si>
+    <t>scrambled_image_prime.jpg</t>
+  </si>
+  <si>
+    <t>scrambled_rubics_image.jpg</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>DSF</t>
+  </si>
+  <si>
+    <t>GSF</t>
+  </si>
+  <si>
+    <t>Entropy</t>
+  </si>
+  <si>
+    <t>Prime Image</t>
+  </si>
+  <si>
+    <t>iteration_0_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_1_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_2_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_3_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_4_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_5_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_6_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_7_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_8_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_9_arnold.jpg</t>
+  </si>
+  <si>
+    <t>prime_res.jpg</t>
   </si>
   <si>
     <t>scrambled_image_prime.jpg</t>
@@ -259,7 +313,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.93359375" customWidth="true"/>
@@ -271,24 +325,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B2" s="0">
         <v>0</v>
@@ -305,7 +359,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="B3" s="0">
         <v>9.4676577601340082</v>
@@ -322,7 +376,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="B4" s="0">
         <v>16.747656089827956</v>
@@ -339,7 +393,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="B5" s="0">
         <v>38.137745658930157</v>
@@ -356,7 +410,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="B6" s="0">
         <v>124.85300397877275</v>
@@ -373,7 +427,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="B7" s="0">
         <v>637.02306843771589</v>
@@ -390,7 +444,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="B8" s="0">
         <v>826.89375509827096</v>
@@ -407,7 +461,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="B9" s="0">
         <v>483.39326596525939</v>
@@ -424,7 +478,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B10" s="0">
         <v>766.10635766312976</v>
@@ -441,7 +495,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="B11" s="0">
         <v>699.33472457175787</v>
@@ -458,35 +512,52 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="B12" s="0">
-        <v>566.76161579289055</v>
+        <v>111.4600213179793</v>
       </c>
       <c r="C12" s="0">
-        <v>7.3247438424006228</v>
+        <v>7.5053322067730859</v>
       </c>
       <c r="D12" s="0">
-        <v>77.376305299864143</v>
+        <v>14.850777853296581</v>
       </c>
       <c r="E12" s="0">
-        <v>0.35858154296875</v>
+        <v>0.3450469970703125</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B13" s="0">
+        <v>566.76161579289055</v>
+      </c>
+      <c r="C13" s="0">
+        <v>7.3247438424006228</v>
+      </c>
+      <c r="D13" s="0">
+        <v>77.376305299864143</v>
+      </c>
+      <c r="E13" s="0">
+        <v>0.35858154296875</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="0">
         <v>7.5430087559069721</v>
       </c>
-      <c r="C13" s="0">
+      <c r="C14" s="0">
         <v>7.542703749578286</v>
       </c>
-      <c r="D13" s="0">
+      <c r="D14" s="0">
         <v>1.0000404372674325</v>
       </c>
-      <c r="E13" s="0">
+      <c r="E14" s="0">
         <v>0.12860107421875</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: fix images problems
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t>Prime Image</t>
   </si>
@@ -196,6 +196,60 @@
   </si>
   <si>
     <t>iteration_9_arnold.jpg</t>
+  </si>
+  <si>
+    <t>scrambled_image_prime.jpg</t>
+  </si>
+  <si>
+    <t>scrambled_rubics_image.jpg</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>DSF</t>
+  </si>
+  <si>
+    <t>GSF</t>
+  </si>
+  <si>
+    <t>Entropy</t>
+  </si>
+  <si>
+    <t>Prime Image</t>
+  </si>
+  <si>
+    <t>iteration_0_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_1_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_2_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_3_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_4_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_5_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_6_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_7_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_8_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_9_arnold.jpg</t>
+  </si>
+  <si>
+    <t>prime_res.jpg</t>
   </si>
   <si>
     <t>scrambled_image_prime.jpg</t>
@@ -325,24 +379,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="B2" s="0">
         <v>0</v>
@@ -359,7 +413,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="B3" s="0">
         <v>9.4676577601340082</v>
@@ -376,7 +430,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="B4" s="0">
         <v>16.747656089827956</v>
@@ -393,7 +447,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="B5" s="0">
         <v>38.137745658930157</v>
@@ -410,7 +464,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="B6" s="0">
         <v>124.85300397877275</v>
@@ -427,7 +481,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="B7" s="0">
         <v>637.02306843771589</v>
@@ -444,7 +498,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="B8" s="0">
         <v>826.89375509827096</v>
@@ -461,7 +515,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="B9" s="0">
         <v>483.39326596525939</v>
@@ -478,7 +532,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="B10" s="0">
         <v>766.10635766312976</v>
@@ -495,7 +549,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="B11" s="0">
         <v>699.33472457175787</v>
@@ -512,7 +566,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="B12" s="0">
         <v>111.4600213179793</v>
@@ -529,7 +583,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="B13" s="0">
         <v>566.76161579289055</v>
@@ -546,7 +600,7 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B14" s="0">
         <v>7.5430087559069721</v>

</xml_diff>

<commit_message>
fix: fix rubics function
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="172">
   <si>
     <t>Prime Image</t>
   </si>
@@ -310,6 +310,213 @@
   </si>
   <si>
     <t>scrambled_rubics_image.jpg</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>DSF</t>
+  </si>
+  <si>
+    <t>GSF</t>
+  </si>
+  <si>
+    <t>Entropy</t>
+  </si>
+  <si>
+    <t>Prime Image</t>
+  </si>
+  <si>
+    <t>iteration_0_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_1_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_2_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_3_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_4_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_5_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_6_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_7_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_8_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_9_arnold.jpg</t>
+  </si>
+  <si>
+    <t>prime_res.jpg</t>
+  </si>
+  <si>
+    <t>scrambled_image_prime.jpg</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>DSF</t>
+  </si>
+  <si>
+    <t>GSF</t>
+  </si>
+  <si>
+    <t>Entropy</t>
+  </si>
+  <si>
+    <t>Prime Image</t>
+  </si>
+  <si>
+    <t>iteration_0_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_1_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_2_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_3_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_4_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_5_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_6_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_7_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_8_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_9_arnold.jpg</t>
+  </si>
+  <si>
+    <t>prime_res.jpg</t>
+  </si>
+  <si>
+    <t>scrambled_image_prime.jpg</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>DSF</t>
+  </si>
+  <si>
+    <t>GSF</t>
+  </si>
+  <si>
+    <t>Entropy</t>
+  </si>
+  <si>
+    <t>Prime Image</t>
+  </si>
+  <si>
+    <t>iteration_0_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_1_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_2_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_3_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_4_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_5_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_6_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_7_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_8_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_9_arnold.jpg</t>
+  </si>
+  <si>
+    <t>prime_res.jpg</t>
+  </si>
+  <si>
+    <t>scrambled_image_prime.jpg</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>DSF</t>
+  </si>
+  <si>
+    <t>GSF</t>
+  </si>
+  <si>
+    <t>Entropy</t>
+  </si>
+  <si>
+    <t>Prime Image</t>
+  </si>
+  <si>
+    <t>iteration_0_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_1_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_2_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_3_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_4_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_5_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_6_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_7_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_8_arnold.jpg</t>
+  </si>
+  <si>
+    <t>iteration_9_arnold.jpg</t>
+  </si>
+  <si>
+    <t>prime_res.jpg</t>
+  </si>
+  <si>
+    <t>rubics.jpg</t>
+  </si>
+  <si>
+    <t>scrambled_image_prime.jpg</t>
   </si>
   <si>
     <t>Efficiency</t>
@@ -370,7 +577,7 @@
   <dimension ref="A1:E14"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.93359375" customWidth="true"/>
+    <col min="1" max="1" width="19.26953125" customWidth="true"/>
     <col min="2" max="2" width="11.7109375" customWidth="true"/>
     <col min="3" max="3" width="11.7109375" customWidth="true"/>
     <col min="4" max="4" width="11.7109375" customWidth="true"/>
@@ -379,24 +586,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>85</v>
+        <v>154</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>99</v>
+        <v>168</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>100</v>
+        <v>169</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>101</v>
+        <v>170</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>102</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>86</v>
+        <v>155</v>
       </c>
       <c r="B2" s="0">
         <v>0</v>
@@ -413,7 +620,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>87</v>
+        <v>156</v>
       </c>
       <c r="B3" s="0">
         <v>9.4676577601340082</v>
@@ -430,7 +637,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>88</v>
+        <v>157</v>
       </c>
       <c r="B4" s="0">
         <v>16.747656089827956</v>
@@ -447,7 +654,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>89</v>
+        <v>158</v>
       </c>
       <c r="B5" s="0">
         <v>38.137745658930157</v>
@@ -464,7 +671,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>90</v>
+        <v>159</v>
       </c>
       <c r="B6" s="0">
         <v>124.85300397877275</v>
@@ -481,7 +688,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>91</v>
+        <v>160</v>
       </c>
       <c r="B7" s="0">
         <v>637.02306843771589</v>
@@ -498,7 +705,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>92</v>
+        <v>161</v>
       </c>
       <c r="B8" s="0">
         <v>826.89375509827096</v>
@@ -515,7 +722,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>93</v>
+        <v>162</v>
       </c>
       <c r="B9" s="0">
         <v>483.39326596525939</v>
@@ -532,7 +739,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>94</v>
+        <v>163</v>
       </c>
       <c r="B10" s="0">
         <v>766.10635766312976</v>
@@ -549,7 +756,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>95</v>
+        <v>164</v>
       </c>
       <c r="B11" s="0">
         <v>699.33472457175787</v>
@@ -566,7 +773,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>96</v>
+        <v>165</v>
       </c>
       <c r="B12" s="0">
         <v>111.4600213179793</v>
@@ -583,36 +790,36 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>97</v>
+        <v>166</v>
       </c>
       <c r="B13" s="0">
-        <v>566.76161579289055</v>
+        <v>8.4218070881881353</v>
       </c>
       <c r="C13" s="0">
-        <v>7.3247438424006228</v>
+        <v>7.4981904775947745</v>
       </c>
       <c r="D13" s="0">
-        <v>77.376305299864143</v>
+        <v>1.1231786006708158</v>
       </c>
       <c r="E13" s="0">
-        <v>0.35858154296875</v>
+        <v>0.1756744384765625</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>98</v>
+        <v>167</v>
       </c>
       <c r="B14" s="0">
-        <v>7.5430087559069721</v>
+        <v>566.76161579289055</v>
       </c>
       <c r="C14" s="0">
-        <v>7.542703749578286</v>
+        <v>7.3247438424006228</v>
       </c>
       <c r="D14" s="0">
-        <v>1.0000404372674325</v>
+        <v>77.376305299864143</v>
       </c>
       <c r="E14" s="0">
-        <v>0.12860107421875</v>
+        <v>0.35858154296875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>